<commit_message>
add summary certain date feature
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7512" uniqueCount="4994">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7512" uniqueCount="4995">
   <si>
     <t>UNA-2010-0066</t>
   </si>
@@ -17550,6 +17550,9 @@
   <si>
     <t>UNA-2016-0181</t>
     <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>24/03/2017</t>
   </si>
 </sst>
 </file>
@@ -18352,8 +18355,8 @@
   <dimension ref="A1:M1491"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1471" sqref="D1471"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -19241,7 +19244,7 @@
         <v>4550</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>4534</v>
+        <v>4994</v>
       </c>
       <c r="F27" s="88" t="s">
         <v>4518</v>
@@ -19272,7 +19275,7 @@
         <v>3905</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>4536</v>
+        <v>4994</v>
       </c>
       <c r="F28" s="88" t="s">
         <v>4518</v>
@@ -19303,7 +19306,7 @@
         <v>4551</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>4536</v>
+        <v>4994</v>
       </c>
       <c r="F29" s="88" t="s">
         <v>4540</v>
@@ -19334,7 +19337,7 @@
         <v>4552</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>4536</v>
+        <v>4994</v>
       </c>
       <c r="F30" s="88" t="s">
         <v>4512</v>
@@ -19365,7 +19368,7 @@
         <v>4553</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>4555</v>
+        <v>4994</v>
       </c>
       <c r="F31" s="88" t="s">
         <v>731</v>
@@ -20204,11 +20207,11 @@
         <v>3352</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" ref="I57:I120" si="2">IF(F57="MB","MA","---")</f>
+        <f t="shared" ref="I57:I65" si="2">IF(F57="MB","MA","---")</f>
         <v>---</v>
       </c>
       <c r="K57" t="str">
-        <f t="shared" ref="K57:K120" si="3">IF(F57="MB","2", IF(F57="","", "1"))</f>
+        <f t="shared" ref="K57:K65" si="3">IF(F57="MB","2", IF(F57="","", "1"))</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ascending and descending, bugs to be fixed.
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7512" uniqueCount="4995">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7524" uniqueCount="4999">
   <si>
     <t>UNA-2010-0066</t>
   </si>
@@ -17553,6 +17553,18 @@
   </si>
   <si>
     <t>24/03/2017</t>
+  </si>
+  <si>
+    <t>2016A-0065</t>
+  </si>
+  <si>
+    <t>2016A-0066</t>
+  </si>
+  <si>
+    <t>17/01/2016</t>
+  </si>
+  <si>
+    <t>16/01/2016</t>
   </si>
 </sst>
 </file>
@@ -18355,8 +18367,8 @@
   <dimension ref="A1:M1491"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27:E31"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -20452,7 +20464,7 @@
         <v>3834</v>
       </c>
       <c r="E65" s="29" t="s">
-        <v>4595</v>
+        <v>4997</v>
       </c>
       <c r="F65" s="89" t="s">
         <v>981</v>
@@ -20470,16 +20482,66 @@
       </c>
     </row>
     <row r="66" spans="1:11">
-      <c r="C66" s="3"/>
-      <c r="D66" s="89"/>
-      <c r="F66" s="89"/>
-      <c r="G66" s="89"/>
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2753</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>4995</v>
+      </c>
+      <c r="D66" s="89" t="s">
+        <v>3834</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>4595</v>
+      </c>
+      <c r="F66" s="89" t="s">
+        <v>981</v>
+      </c>
+      <c r="G66" s="89" t="s">
+        <v>685</v>
+      </c>
+      <c r="I66" t="str">
+        <f t="shared" ref="I66:I67" si="4">IF(F66="MB","MA","---")</f>
+        <v>---</v>
+      </c>
+      <c r="K66" t="str">
+        <f t="shared" ref="K66:K67" si="5">IF(F66="MB","2", IF(F66="","", "1"))</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="1:11">
-      <c r="C67" s="3"/>
-      <c r="D67" s="89"/>
-      <c r="F67" s="89"/>
-      <c r="G67" s="89"/>
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>2753</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>4996</v>
+      </c>
+      <c r="D67" s="89" t="s">
+        <v>3834</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>4998</v>
+      </c>
+      <c r="F67" s="89" t="s">
+        <v>981</v>
+      </c>
+      <c r="G67" s="89" t="s">
+        <v>685</v>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" si="4"/>
+        <v>---</v>
+      </c>
+      <c r="K67" t="str">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="68" spans="1:11">
       <c r="C68" s="3"/>

</xml_diff>